<commit_message>
excel actualizado y traspasaddo al word
</commit_message>
<xml_diff>
--- a/Trabajos Prácticos/TP_12/Recursos/DeliverEat_Template_Caso_De_Prueba_Defectos.xlsx
+++ b/Trabajos Prácticos/TP_12/Recursos/DeliverEat_Template_Caso_De_Prueba_Defectos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\Trabajos Prácticos\TP_12\Recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gonza\Documents\2022\ISW\Repositorio\Repositorio_Grupo2_ISW\Trabajos Prácticos\TP_12\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E1577D-E0A2-41FB-BB2F-D9F07CABBE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325B0DC-F24B-43A0-8C7F-3B5DC24A39F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="-120" windowWidth="28320" windowHeight="16440" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clases de Equivalencia" sheetId="29" r:id="rId1"/>
@@ -495,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -989,17 +989,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1017,7 +1006,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1174,8 +1163,32 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1183,41 +1196,23 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1668,11 +1663,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAD9840-36E0-4F21-9FAD-A2DDF0698138}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -1685,26 +1680,26 @@
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="63"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="16"/>
@@ -1717,7 +1712,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="28"/>
       <c r="C4" s="29"/>
       <c r="D4" s="30"/>
@@ -1726,7 +1721,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="16"/>
@@ -1739,7 +1734,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="28"/>
       <c r="C6" s="29" t="s">
         <v>39</v>
@@ -1750,7 +1745,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="56" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="16"/>
@@ -1763,7 +1758,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="28"/>
       <c r="C8" s="29" t="s">
         <v>41</v>
@@ -1774,7 +1769,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="58" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="16"/>
@@ -1787,7 +1782,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="28"/>
       <c r="C10" s="29" t="s">
         <v>41</v>
@@ -1798,7 +1793,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="56" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="16"/>
@@ -1809,7 +1804,7 @@
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="28"/>
       <c r="C12" s="29" t="s">
         <v>31</v>
@@ -1818,7 +1813,7 @@
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="58" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="16"/>
@@ -1832,7 +1827,7 @@
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="28"/>
       <c r="C14" s="29" t="s">
         <v>38</v>
@@ -1841,7 +1836,7 @@
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="56" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="16"/>
@@ -1854,7 +1849,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="28"/>
       <c r="C16" s="29"/>
       <c r="D16" s="30"/>
@@ -1863,7 +1858,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="58" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="16"/>
@@ -1876,7 +1871,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
       <c r="D18" s="30"/>
@@ -1885,7 +1880,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="56" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="16"/>
@@ -1896,7 +1891,7 @@
       <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="28"/>
       <c r="C20" s="29" t="s">
         <v>31</v>
@@ -1918,7 +1913,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="56" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="32"/>
@@ -1931,7 +1926,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
+      <c r="A23" s="57"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22" t="s">
         <v>45</v>
@@ -1955,7 +1950,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="56" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="16"/>
@@ -1968,7 +1963,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="38"/>
       <c r="C26" s="39"/>
       <c r="D26" s="40"/>
@@ -1977,7 +1972,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="58" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="16"/>
@@ -1990,7 +1985,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="67"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
       <c r="D28" s="30"/>
@@ -1999,7 +1994,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="44"/>
       <c r="C29" s="45"/>
       <c r="D29" s="46"/>
@@ -2008,7 +2003,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="56" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="16"/>
@@ -2021,7 +2016,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="68"/>
+      <c r="A31" s="66"/>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
       <c r="D31" s="43"/>
@@ -2030,7 +2025,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="68"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="25"/>
       <c r="C32" s="26"/>
       <c r="D32" s="27"/>
@@ -2039,7 +2034,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="68"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
       <c r="D33" s="43"/>
@@ -2048,7 +2043,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
+      <c r="A34" s="57"/>
       <c r="B34" s="21"/>
       <c r="C34" s="22"/>
       <c r="D34" s="23"/>
@@ -2070,7 +2065,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="56" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="16"/>
@@ -2083,7 +2078,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="68"/>
+      <c r="A37" s="66"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
       <c r="D37" s="43"/>
@@ -2092,7 +2087,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="68"/>
+      <c r="A38" s="66"/>
       <c r="B38" s="25"/>
       <c r="C38" s="26"/>
       <c r="D38" s="27"/>
@@ -2101,7 +2096,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="28"/>
       <c r="C39" s="29"/>
       <c r="D39" s="30"/>
@@ -2110,7 +2105,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="58" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="16"/>
@@ -2123,7 +2118,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="67"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
       <c r="D41" s="43"/>
@@ -2132,7 +2127,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="21"/>
       <c r="C42" s="22"/>
       <c r="D42" s="23"/>
@@ -2154,7 +2149,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="58" t="s">
         <v>18</v>
       </c>
       <c r="B44" s="16"/>
@@ -2167,7 +2162,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="67"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
       <c r="D45" s="43"/>
@@ -2176,7 +2171,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="67"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="25"/>
       <c r="C46" s="26"/>
       <c r="D46" s="27"/>
@@ -2185,7 +2180,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="67"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="41"/>
       <c r="C47" s="42"/>
       <c r="D47" s="43"/>
@@ -2194,7 +2189,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="61"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="21"/>
       <c r="C48" s="22"/>
       <c r="D48" s="23"/>
@@ -2203,16 +2198,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
-      <c r="E49" s="66"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="62"/>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="25"/>
@@ -2225,7 +2220,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="56"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="41"/>
       <c r="C51" s="42"/>
       <c r="D51" s="43"/>
@@ -2234,7 +2229,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="56"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="25"/>
       <c r="C52" s="26"/>
       <c r="D52" s="27"/>
@@ -2243,7 +2238,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="56"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="41"/>
       <c r="C53" s="42"/>
       <c r="D53" s="43"/>
@@ -2252,7 +2247,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="56"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="25"/>
       <c r="C54" s="26"/>
       <c r="D54" s="27"/>
@@ -2261,7 +2256,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="56"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="41"/>
       <c r="C55" s="42"/>
       <c r="D55" s="43"/>
@@ -2270,7 +2265,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="56"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="25"/>
       <c r="C56" s="26"/>
       <c r="D56" s="27"/>
@@ -2279,7 +2274,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="56"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="41"/>
       <c r="C57" s="42"/>
       <c r="D57" s="43"/>
@@ -2288,7 +2283,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="56"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="25"/>
       <c r="C58" s="26"/>
       <c r="D58" s="27"/>
@@ -2297,7 +2292,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="56"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="41"/>
       <c r="C59" s="42"/>
       <c r="D59" s="43"/>
@@ -2306,7 +2301,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="56"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="25"/>
       <c r="C60" s="26"/>
       <c r="D60" s="27"/>
@@ -2315,7 +2310,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="56"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="41"/>
       <c r="C61" s="42"/>
       <c r="D61" s="43"/>
@@ -2324,7 +2319,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="56"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="41"/>
       <c r="C62" s="42"/>
       <c r="D62" s="43"/>
@@ -2333,7 +2328,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="56"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="25"/>
       <c r="C63" s="26"/>
       <c r="D63" s="27"/>
@@ -2342,7 +2337,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="56"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="41"/>
       <c r="C64" s="42"/>
       <c r="D64" s="43"/>
@@ -2351,7 +2346,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="56"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="25"/>
       <c r="C65" s="26"/>
       <c r="D65" s="27"/>
@@ -2360,7 +2355,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="56"/>
+      <c r="A66" s="64"/>
       <c r="B66" s="51"/>
       <c r="C66" s="52"/>
       <c r="D66" s="53"/>
@@ -2369,7 +2364,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="56"/>
+      <c r="A67" s="64"/>
       <c r="B67" s="48"/>
       <c r="C67" s="49"/>
       <c r="D67" s="50"/>
@@ -2378,7 +2373,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="56"/>
+      <c r="A68" s="64"/>
       <c r="B68" s="51"/>
       <c r="C68" s="52"/>
       <c r="D68" s="53"/>
@@ -2387,7 +2382,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="56"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="48"/>
       <c r="C69" s="49"/>
       <c r="D69" s="50"/>
@@ -2396,7 +2391,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="56"/>
+      <c r="A70" s="64"/>
       <c r="B70" s="51"/>
       <c r="C70" s="52"/>
       <c r="D70" s="53"/>
@@ -2405,7 +2400,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="56"/>
+      <c r="A71" s="64"/>
       <c r="B71" s="48"/>
       <c r="C71" s="49"/>
       <c r="D71" s="50"/>
@@ -2414,7 +2409,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="56"/>
+      <c r="A72" s="64"/>
       <c r="B72" s="51"/>
       <c r="C72" s="52"/>
       <c r="D72" s="53"/>
@@ -2423,7 +2418,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="56"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="48"/>
       <c r="C73" s="49"/>
       <c r="D73" s="50"/>
@@ -2432,7 +2427,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="56"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="51"/>
       <c r="C74" s="52"/>
       <c r="D74" s="53"/>
@@ -2441,7 +2436,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="56"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="48"/>
       <c r="C75" s="49"/>
       <c r="D75" s="50"/>
@@ -2450,7 +2445,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="56"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="51"/>
       <c r="C76" s="52"/>
       <c r="D76" s="53"/>
@@ -2459,7 +2454,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="56"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="48"/>
       <c r="C77" s="49"/>
       <c r="D77" s="50"/>
@@ -2468,32 +2463,29 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="57"/>
-      <c r="B78" s="28"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="29" t="s">
+      <c r="A78" s="64"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="53"/>
+      <c r="E78" s="52" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="79" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="C79" t="s">
+      <c r="B79" s="68"/>
+      <c r="C79" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="54" t="s">
+      <c r="D79" s="70"/>
+      <c r="E79" s="19" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A2:E2"/>
     <mergeCell ref="A50:A78"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
@@ -2510,6 +2502,11 @@
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2523,7 +2520,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.140625" customWidth="1"/>
@@ -2783,15 +2780,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -2917,6 +2905,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
@@ -2930,14 +2927,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2954,4 +2943,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>